<commit_message>
added Sarima Model for West Bengal
</commit_message>
<xml_diff>
--- a/West Bengal/Future_Predicted_WB.xlsx
+++ b/West Bengal/Future_Predicted_WB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karti\Desktop\Arima &amp; Sarima - COVID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karti\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{91E45CF9-7C57-45B5-BAA3-90AE15B34218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{3590EEB5-1DA5-4B01-AA33-E566964D8DCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,22 +171,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>137159</xdr:rowOff>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>327512</xdr:colOff>
+      <xdr:colOff>269565</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24C0EDB4-C656-4EEE-9278-6B66BB3FE5F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EAECD8B-F1F8-4985-A60E-DC43D6648A90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -202,8 +202,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="68580" y="4663439"/>
-          <a:ext cx="6857852" cy="4564381"/>
+          <a:off x="0" y="4678681"/>
+          <a:ext cx="6868485" cy="4655819"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -215,22 +215,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
+      <xdr:colOff>266715</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>115821</xdr:rowOff>
+      <xdr:rowOff>160022</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>182676</xdr:colOff>
+      <xdr:colOff>182893</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA70E2CD-A28E-45D2-A6F9-02B2CF99A7B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46468666-86EA-4601-8644-9E78E01DB7C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -246,8 +246,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6896100" y="4642101"/>
-          <a:ext cx="7017816" cy="4593339"/>
+          <a:off x="6865635" y="4686302"/>
+          <a:ext cx="7048498" cy="4587238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -259,22 +259,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:colOff>1424955</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>62481</xdr:rowOff>
+      <xdr:rowOff>22862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>162552</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228006</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>7619</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44AB1361-DBCE-4BB5-9958-F9626B09BEA8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84F7147C-2D6F-4642-8FE6-3B54DD01E421}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -290,8 +290,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3611880" y="9282681"/>
-          <a:ext cx="6629400" cy="4458711"/>
+          <a:off x="3817635" y="9243062"/>
+          <a:ext cx="6971691" cy="4678677"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -630,13 +630,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>872.55044867092101</v>
+        <v>570.97052747590601</v>
       </c>
       <c r="C2">
-        <v>317.68708134396002</v>
+        <v>713.92759538233497</v>
       </c>
       <c r="D2">
-        <v>14.491686636061299</v>
+        <v>13.974615576801201</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -644,13 +644,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>841.86464186913804</v>
+        <v>537.14491254978702</v>
       </c>
       <c r="C3">
-        <v>318.86379779938198</v>
+        <v>595.85234084363697</v>
       </c>
       <c r="D3">
-        <v>15.929711026914701</v>
+        <v>14.196198166060899</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -658,13 +658,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>870.81890636939602</v>
+        <v>551.71371859295698</v>
       </c>
       <c r="C4">
-        <v>343.95277268762999</v>
+        <v>776.79182338947896</v>
       </c>
       <c r="D4">
-        <v>14.7713999855272</v>
+        <v>15.0160713820236</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -672,13 +672,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>881.67401658875599</v>
+        <v>550.73712897996995</v>
       </c>
       <c r="C5">
-        <v>347.564437026441</v>
+        <v>673.85185481942005</v>
       </c>
       <c r="D5">
-        <v>16.2094243763806</v>
+        <v>12.904359145672499</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,13 +686,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>828.08613578623601</v>
+        <v>599.21430853262996</v>
       </c>
       <c r="C6">
-        <v>335.28598605712398</v>
+        <v>652.52588889414403</v>
       </c>
       <c r="D6">
-        <v>15.051113334993</v>
+        <v>15.0231788200111</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -700,13 +700,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>859.87772272659697</v>
+        <v>689.02704945130097</v>
       </c>
       <c r="C7">
-        <v>363.70467241320102</v>
+        <v>756.80137373201001</v>
       </c>
       <c r="D7">
-        <v>16.489137725846501</v>
+        <v>15.865033395928499</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -714,13 +714,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>916.093253736581</v>
+        <v>603.84563365344695</v>
       </c>
       <c r="C8">
-        <v>363.162731480876</v>
+        <v>717.22786579998001</v>
       </c>
       <c r="D8">
-        <v>15.3308266844589</v>
+        <v>15.199292653665699</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -728,13 +728,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>946.11112471196304</v>
+        <v>568.08834587666502</v>
       </c>
       <c r="C9">
-        <v>391.41202973705299</v>
+        <v>727.45041807895996</v>
       </c>
       <c r="D9">
-        <v>16.768851075312401</v>
+        <v>22.578353926055399</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -742,13 +742,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>1029.87090832588</v>
+        <v>619.701840439325</v>
       </c>
       <c r="C10">
-        <v>375.745502831674</v>
+        <v>721.23356532594198</v>
       </c>
       <c r="D10">
-        <v>15.610540033924799</v>
+        <v>15.5494851737521</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -756,13 +756,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>1009.1115917012499</v>
+        <v>575.80054364554906</v>
       </c>
       <c r="C11">
-        <v>368.22395176355099</v>
+        <v>708.85007271650295</v>
       </c>
       <c r="D11">
-        <v>17.048564424778299</v>
+        <v>15.8749236960519</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -770,13 +770,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>1038.00573420453</v>
+        <v>643.70656582884305</v>
       </c>
       <c r="C12">
-        <v>369.40066821897398</v>
+        <v>703.29421143199602</v>
       </c>
       <c r="D12">
-        <v>15.8902533833907</v>
+        <v>14.978982212655801</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -784,13 +784,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>1037.9345981009201</v>
+        <v>615.28196141413002</v>
       </c>
       <c r="C13">
-        <v>394.48964310722101</v>
+        <v>697.60365537582402</v>
       </c>
       <c r="D13">
-        <v>17.328277774244199</v>
+        <v>14.648577109004799</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -798,13 +798,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>984.081849096376</v>
+        <v>550.32428818430503</v>
       </c>
       <c r="C14">
-        <v>398.10130744603202</v>
+        <v>746.02097621540202</v>
       </c>
       <c r="D14">
-        <v>16.169966732856601</v>
+        <v>15.549454745393</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -812,13 +812,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>996.42133620449795</v>
+        <v>623.56309712284997</v>
       </c>
       <c r="C15">
-        <v>385.822856476715</v>
+        <v>748.05528526823696</v>
       </c>
       <c r="D15">
-        <v>17.607991123710001</v>
+        <v>15.851043252694399</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -826,13 +826,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>1079.8908080697699</v>
+        <v>615.42703494919704</v>
       </c>
       <c r="C16">
-        <v>414.24154283279199</v>
+        <v>825.15435804017295</v>
       </c>
       <c r="D16">
-        <v>16.449680082322502</v>
+        <v>16.6820448500008</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -840,13 +840,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>1116.08437518495</v>
+        <v>615.50347778398998</v>
       </c>
       <c r="C17">
-        <v>413.69960190046697</v>
+        <v>947.43457362579704</v>
       </c>
       <c r="D17">
-        <v>17.887704473175901</v>
+        <v>14.568850369013299</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -854,13 +854,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>1201.3816512373</v>
+        <v>584.09636159977094</v>
       </c>
       <c r="C18">
-        <v>441.94890015664402</v>
+        <v>895.44155799361295</v>
       </c>
       <c r="D18">
-        <v>16.729393431788399</v>
+        <v>16.6889693235936</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -868,13 +868,13 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>1179.4128472224299</v>
+        <v>595.06066997875496</v>
       </c>
       <c r="C19">
-        <v>426.28237325126599</v>
+        <v>962.99917562641997</v>
       </c>
       <c r="D19">
-        <v>18.167417822641799</v>
+        <v>17.5306602044286</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -882,13 +882,13 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>1209.25223211922</v>
+        <v>618.35205398143501</v>
       </c>
       <c r="C20">
-        <v>418.76082218314298</v>
+        <v>946.74052316965594</v>
       </c>
       <c r="D20">
-        <v>17.0091067812543</v>
+        <v>16.865283879016602</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,13 +896,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>1213.7967515707801</v>
+        <v>664.36720166437203</v>
       </c>
       <c r="C21">
-        <v>419.937538638565</v>
+        <v>941.64417143675405</v>
       </c>
       <c r="D21">
-        <v>18.447131172107699</v>
+        <v>24.252371488792502</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -910,13 +910,13 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>1153.00198337448</v>
+        <v>802.767955863917</v>
       </c>
       <c r="C22">
-        <v>445.02651352681198</v>
+        <v>833.58488311223698</v>
       </c>
       <c r="D22">
-        <v>17.288820130720101</v>
+        <v>17.2115065736064</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -924,13 +924,13 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>1175.57936445053</v>
+        <v>694.71949971232596</v>
       </c>
       <c r="C23">
-        <v>448.63817786562402</v>
+        <v>996.99691729966196</v>
       </c>
       <c r="D23">
-        <v>18.7268445215736</v>
+        <v>17.5383867847791</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -938,13 +938,13 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>1259.28193796849</v>
+        <v>662.74895556520096</v>
       </c>
       <c r="C24">
-        <v>436.359726896307</v>
+        <v>899.63328778782</v>
       </c>
       <c r="D24">
-        <v>17.568533480186002</v>
+        <v>16.644733899451001</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -952,13 +952,13 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>1296.6338143614801</v>
+        <v>727.33775580214603</v>
       </c>
       <c r="C25">
-        <v>464.77841325238302</v>
+        <v>883.71730637973997</v>
       </c>
       <c r="D25">
-        <v>19.006557871039501</v>
+        <v>16.3139694120527</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -966,13 +966,13 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>1383.32968877804</v>
+        <v>625.13951651890204</v>
       </c>
       <c r="C26">
-        <v>464.23647232005902</v>
+        <v>980.22727261043894</v>
       </c>
       <c r="D26">
-        <v>17.848246829651899</v>
+        <v>17.211476113115602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>